<commit_message>
relative css sizing and positioning
Changed css sizing and positive to be relative so it will scale and
gave depth to buttons, added status/header bar, and additional buttons
</commit_message>
<xml_diff>
--- a/IS322 JS Sudoku Task List.xlsx
+++ b/IS322 JS Sudoku Task List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>PhoneGAP Deployment???</t>
+  </si>
+  <si>
+    <t>Brian Galok</t>
   </si>
 </sst>
 </file>
@@ -495,9 +498,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+    <sheetView windowProtection="1" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -538,6 +541,9 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="60">
       <c r="A3" s="1" t="s">
@@ -560,6 +566,9 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="75">
       <c r="A5" s="1" t="s">
@@ -598,6 +607,9 @@
       </c>
       <c r="C7" t="s">
         <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="150">

</xml_diff>